<commit_message>
Dropdown z metodami interpolacji oraz interpolacja liniowa
</commit_message>
<xml_diff>
--- a/src/excel_datas/data2.xlsx
+++ b/src/excel_datas/data2.xlsx
@@ -35,13 +35,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -57,6 +56,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,7 +127,417 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$367:$E$375</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$367:$F$375</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="62530374"/>
+        <c:axId val="91783935"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="62530374"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91783935"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="91783935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="62530374"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>479880</xdr:colOff>
+      <xdr:row>384</xdr:row>
+      <xdr:rowOff>120960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4593240" y="64181160"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -131,15 +545,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2001"/>
+  <dimension ref="A1:F2001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1986" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1997" activeCellId="0" sqref="F1997"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A365" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E367" activeCellId="0" sqref="E367"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3074,6 +3488,12 @@
       <c r="B367" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E367" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F367" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="1" t="n">
@@ -3082,6 +3502,12 @@
       <c r="B368" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="E368" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F368" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="1" t="n">
@@ -3090,6 +3516,12 @@
       <c r="B369" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E369" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F369" s="0" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="1" t="n">
@@ -3098,6 +3530,12 @@
       <c r="B370" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="E370" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F370" s="0" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="1" t="n">
@@ -3106,6 +3544,12 @@
       <c r="B371" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="E371" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F371" s="0" t="n">
+        <v>126</v>
+      </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="1" t="n">
@@ -3114,6 +3558,12 @@
       <c r="B372" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="E372" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F372" s="0" t="n">
+        <v>127</v>
+      </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="1" t="n">
@@ -3122,6 +3572,12 @@
       <c r="B373" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E373" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F373" s="0" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="1" t="n">
@@ -3130,6 +3586,12 @@
       <c r="B374" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E374" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F374" s="0" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="n">
@@ -3138,6 +3600,12 @@
       <c r="B375" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E375" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F375" s="0" t="n">
+        <v>130</v>
+      </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="n">
@@ -3146,6 +3614,12 @@
       <c r="B376" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="E376" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F376" s="0" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="1" t="n">
@@ -3154,6 +3628,12 @@
       <c r="B377" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E377" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F377" s="0" t="n">
+        <v>132</v>
+      </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="1" t="n">
@@ -3162,6 +3642,12 @@
       <c r="B378" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="E378" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F378" s="0" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="1" t="n">
@@ -3170,6 +3656,12 @@
       <c r="B379" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="E379" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F379" s="0" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="1" t="n">
@@ -3178,6 +3670,12 @@
       <c r="B380" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="E380" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F380" s="0" t="n">
+        <v>135</v>
+      </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="1" t="n">
@@ -3186,6 +3684,12 @@
       <c r="B381" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E381" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F381" s="0" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="1" t="n">
@@ -3194,6 +3698,12 @@
       <c r="B382" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E382" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F382" s="0" t="n">
+        <v>137</v>
+      </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="1" t="n">
@@ -3202,6 +3712,12 @@
       <c r="B383" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E383" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F383" s="0" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="1" t="n">
@@ -3210,6 +3726,12 @@
       <c r="B384" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="E384" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F384" s="0" t="n">
+        <v>139</v>
+      </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="1" t="n">
@@ -3217,6 +3739,12 @@
       </c>
       <c r="B385" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="E385" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F385" s="0" t="n">
+        <v>140</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16155,5 +16683,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>